<commit_message>
documentation updates; separated seam component; source code archives; added speedup graph to energy test; fixed energy parallel function for combined program;
</commit_message>
<xml_diff>
--- a/documents/energy_parallel_test.xlsx
+++ b/documents/energy_parallel_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Number of</t>
   </si>
@@ -57,6 +57,9 @@
   <si>
     <t>Individual</t>
   </si>
+  <si>
+    <t>Speedup</t>
+  </si>
 </sst>
 </file>
 
@@ -65,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,6 +89,24 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -294,6 +315,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -351,11 +373,331 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48768896"/>
-        <c:axId val="44988565"/>
+        <c:axId val="75920728"/>
+        <c:axId val="98981484"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48768896"/>
+        <c:axId val="75920728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Number of Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98981484"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98981484"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Runtime (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75920728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Number of Processors vs. Speedup Factor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.43977430574681</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.33565288161292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.06823707393625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65312421490866</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.649469949339571</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="48489076"/>
+        <c:axId val="48524708"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="48489076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,12 +770,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44988565"/>
+        <c:crossAx val="48524708"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44988565"/>
+        <c:axId val="48524708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +821,7 @@
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Runtime (s)</a:t>
+                  <a:t>Speedup Factor</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -515,7 +857,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48768896"/>
+        <c:crossAx val="48489076"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -547,15 +889,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>712800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
+      <xdr:colOff>71280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -563,12 +905,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2286000" y="2302200"/>
+        <a:off x="2274840" y="2293200"/>
+        <a:ext cx="5606640" cy="3239280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>486720</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>83880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>779040</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>72360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1267560" y="5773320"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -582,16 +954,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -638,6 +1007,9 @@
       <c r="I2" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -676,6 +1048,10 @@
       <c r="K3" s="0" t="n">
         <v>332.864</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">479.214/H3</f>
+        <v>1.43977430574681</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -714,6 +1090,10 @@
       <c r="K4" s="0" t="n">
         <v>359.558</v>
       </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">479.214/H4</f>
+        <v>1.33565288161292</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -752,6 +1132,10 @@
       <c r="K5" s="0" t="n">
         <v>356.572</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">479.214/H5</f>
+        <v>1.06823707393625</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -790,6 +1174,10 @@
       <c r="K6" s="0" t="n">
         <v>767.93</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">479.214/H6</f>
+        <v>0.65312421490866</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -827,6 +1215,10 @@
       </c>
       <c r="K7" s="0" t="n">
         <v>752.11</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">479.214/H7</f>
+        <v>0.649469949339571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>